<commit_message>
update data till Nov 2023
</commit_message>
<xml_diff>
--- a/data-raw/unhcr_2022/iati_location.xlsx
+++ b/data-raw/unhcr_2022/iati_location.xlsx
@@ -12622,7 +12622,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>BIHp000058</t>
+          <t>BIHp004115</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -12664,7 +12664,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>BIHp004115</t>
+          <t>BIHp000058</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">

</xml_diff>